<commit_message>
modification MCD/MLD, regénération du script SQL et ajout manuel des "AUTO_INCREMENT"
</commit_message>
<xml_diff>
--- a/Dictionnaire de données.xlsx
+++ b/Dictionnaire de données.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.tamanini\Documents\GitHub\MOMAS_TAMANINI_Gestion_boutique_en_ligne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAD0264-EBAF-47F9-8874-1AECDC003900}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDC101D-3485-40AA-AF64-AB9B2E82B3A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{D5C6E89A-C8D6-422B-A012-B6E286694171}"/>
+    <workbookView xWindow="2496" yWindow="348" windowWidth="17280" windowHeight="8964" xr2:uid="{D5C6E89A-C8D6-422B-A012-B6E286694171}"/>
   </bookViews>
   <sheets>
     <sheet name="vetement" sheetId="1" r:id="rId1"/>
-    <sheet name="utilisateur" sheetId="2" r:id="rId2"/>
-    <sheet name="commande" sheetId="3" r:id="rId3"/>
-    <sheet name="categorie" sheetId="4" r:id="rId4"/>
-    <sheet name="taille" sheetId="5" r:id="rId5"/>
-    <sheet name="couleur" sheetId="6" r:id="rId6"/>
+    <sheet name="declinaison_vetement" sheetId="7" r:id="rId2"/>
+    <sheet name="utilisateur" sheetId="2" r:id="rId3"/>
+    <sheet name="commande" sheetId="3" r:id="rId4"/>
+    <sheet name="categorie" sheetId="4" r:id="rId5"/>
+    <sheet name="taille" sheetId="5" r:id="rId6"/>
+    <sheet name="couleur" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="72">
   <si>
     <t>NOM CODE</t>
   </si>
@@ -101,18 +102,6 @@
     <t>DESCRIPTION_VETEMENT</t>
   </si>
   <si>
-    <t>prix_vetement</t>
-  </si>
-  <si>
-    <t>PRIX_VETEMENT</t>
-  </si>
-  <si>
-    <t>quantite_vetement</t>
-  </si>
-  <si>
-    <t>QUANTITE_VETEMENT</t>
-  </si>
-  <si>
     <t>A200</t>
   </si>
   <si>
@@ -182,12 +171,6 @@
     <t>PRIX_COMMANDE</t>
   </si>
   <si>
-    <t>quantite_commandee</t>
-  </si>
-  <si>
-    <t>QUANTITE_COMMANDEE</t>
-  </si>
-  <si>
     <t>Entité : commande</t>
   </si>
   <si>
@@ -197,9 +180,6 @@
     <t>&gt;=2 et &lt;=2000</t>
   </si>
   <si>
-    <t>&gt;=1 et &lt;=20</t>
-  </si>
-  <si>
     <t>Première Lettre Majuscule</t>
   </si>
   <si>
@@ -246,23 +226,46 @@
   </si>
   <si>
     <t>NOM_COULEUR</t>
+  </si>
+  <si>
+    <t>id_declinaison</t>
+  </si>
+  <si>
+    <t>ID_DECLINAISON</t>
+  </si>
+  <si>
+    <t>prix_declinaison</t>
+  </si>
+  <si>
+    <t>PRIX_DECLINAISON</t>
+  </si>
+  <si>
+    <t>quantite_declinaison</t>
+  </si>
+  <si>
+    <t>QUANTITE_DECLINAISON</t>
+  </si>
+  <si>
+    <t>mdp_utilisateur</t>
+  </si>
+  <si>
+    <t>MDP_UTILISATEUR</t>
+  </si>
+  <si>
+    <t>Entité : declinaison_vetement</t>
+  </si>
+  <si>
+    <t>999999.99</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -357,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -374,9 +377,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -697,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498533F2-0DA1-4E77-91A1-CB571189B156}">
-  <dimension ref="C5:I11"/>
+  <dimension ref="C5:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,7 +771,7 @@
         <v>9</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
@@ -785,7 +785,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>11</v>
@@ -794,7 +794,7 @@
         <v>9</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
@@ -808,7 +808,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>11</v>
@@ -817,53 +817,7 @@
         <v>9</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="8">
-        <v>999999</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -873,11 +827,135 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4304FFD5-C1EC-4826-B151-068C11706822}">
-  <dimension ref="C5:I11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36043036-6299-4A65-803C-61D703A1AD81}">
+  <dimension ref="B3:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="7">
+        <v>999999</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7">
+        <v>999999</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4304FFD5-C1EC-4826-B151-068C11706822}">
+  <dimension ref="C5:I12"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -893,7 +971,7 @@
   <sheetData>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="3"/>
@@ -927,10 +1005,10 @@
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>7</v>
@@ -945,21 +1023,21 @@
         <v>9</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>11</v>
@@ -968,21 +1046,21 @@
         <v>9</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>11</v>
@@ -991,21 +1069,21 @@
         <v>9</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>11</v>
@@ -1017,21 +1095,41 @@
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="10" t="s">
+      <c r="F11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1040,12 +1138,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C123B1-66C5-4D76-B737-02B0B32BCA76}">
-  <dimension ref="C5:I10"/>
+  <dimension ref="C5:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,7 +1159,7 @@
   <sheetData>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="3"/>
@@ -1095,10 +1193,10 @@
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>7</v>
@@ -1113,21 +1211,21 @@
         <v>9</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>11</v>
@@ -1136,15 +1234,15 @@
         <v>9</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>7</v>
@@ -1159,30 +1257,7 @@
         <v>9</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="7">
-        <v>999999</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1190,7 +1265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BA3E90-DE6D-4D48-9BB2-A805CEC22257}">
   <dimension ref="C5:I8"/>
   <sheetViews>
@@ -1211,7 +1286,7 @@
   <sheetData>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="3"/>
@@ -1245,10 +1320,10 @@
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>7</v>
@@ -1263,21 +1338,21 @@
         <v>9</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>11</v>
@@ -1286,7 +1361,7 @@
         <v>9</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1294,7 +1369,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79BB9C3D-B907-498C-B079-B831CD72AE12}">
   <dimension ref="C5:I8"/>
   <sheetViews>
@@ -1315,7 +1390,7 @@
   <sheetData>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="3"/>
@@ -1349,10 +1424,10 @@
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>7</v>
@@ -1367,21 +1442,21 @@
         <v>9</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>11</v>
@@ -1390,7 +1465,7 @@
         <v>9</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1398,11 +1473,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A21DD5E-8E20-4671-922D-9C4DC0D68662}">
   <dimension ref="C5:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -1419,7 +1494,7 @@
   <sheetData>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="3"/>
@@ -1453,10 +1528,10 @@
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>7</v>
@@ -1471,21 +1546,21 @@
         <v>9</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>11</v>
@@ -1494,7 +1569,7 @@
         <v>9</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>